<commit_message>
Good version for the ratings.
Maybe some more fine tuning needed
</commit_message>
<xml_diff>
--- a/2024-2025/output_rp_excel.xlsx
+++ b/2024-2025/output_rp_excel.xlsx
@@ -588,7 +588,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>1.4</v>
+        <v>2.9</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -676,7 +676,7 @@
         <v>5</v>
       </c>
       <c r="F3" t="n">
-        <v>2.4</v>
+        <v>3.3</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
@@ -848,7 +848,7 @@
         <v>15</v>
       </c>
       <c r="F5" t="n">
-        <v>4.4</v>
+        <v>4.2</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -936,7 +936,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>3.606523859504144</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1024,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
@@ -1108,7 +1108,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1196,7 +1196,7 @@
         <v>9</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>3.567258560469176</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
@@ -1280,7 +1280,7 @@
         <v>8</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1368,7 +1368,7 @@
         <v>8</v>
       </c>
       <c r="F11" t="n">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1456,7 +1456,7 @@
         <v>6</v>
       </c>
       <c r="F12" t="n">
-        <v>2.2</v>
+        <v>3</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
@@ -1540,7 +1540,7 @@
         <v>6</v>
       </c>
       <c r="F13" t="n">
-        <v>2.2</v>
+        <v>3.1</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
@@ -1624,7 +1624,7 @@
         <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
@@ -1708,7 +1708,7 @@
         <v>5</v>
       </c>
       <c r="F15" t="n">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1796,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
@@ -1880,7 +1880,7 @@
         <v>24</v>
       </c>
       <c r="F17" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
@@ -1964,7 +1964,7 @@
         <v>13</v>
       </c>
       <c r="F18" t="n">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -2052,7 +2052,7 @@
         <v>12</v>
       </c>
       <c r="F19" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -2224,7 +2224,7 @@
         <v>9</v>
       </c>
       <c r="F21" t="n">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
@@ -2308,7 +2308,7 @@
         <v>9</v>
       </c>
       <c r="F22" t="n">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -2396,7 +2396,7 @@
         <v>3</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
@@ -2480,7 +2480,7 @@
         <v>27</v>
       </c>
       <c r="F24" t="n">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -2568,7 +2568,7 @@
         <v>24</v>
       </c>
       <c r="F25" t="n">
-        <v>4.6</v>
+        <v>3.8</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -2656,7 +2656,7 @@
         <v>15</v>
       </c>
       <c r="F26" t="n">
-        <v>3</v>
+        <v>3.131638309798655</v>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
@@ -2740,7 +2740,7 @@
         <v>13</v>
       </c>
       <c r="F27" t="n">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
         <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
@@ -2912,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
@@ -2996,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
@@ -3080,7 +3080,7 @@
         <v>15</v>
       </c>
       <c r="F31" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
@@ -3164,7 +3164,7 @@
         <v>7</v>
       </c>
       <c r="F32" t="n">
-        <v>1.7</v>
+        <v>2.9</v>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
@@ -3248,7 +3248,7 @@
         <v>7</v>
       </c>
       <c r="F33" t="n">
-        <v>4</v>
+        <v>3.567258560469176</v>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
@@ -3332,7 +3332,7 @@
         <v>6</v>
       </c>
       <c r="F34" t="n">
-        <v>4</v>
+        <v>3.567258560469176</v>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
@@ -3416,7 +3416,7 @@
         <v>5</v>
       </c>
       <c r="F35" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
@@ -3500,7 +3500,7 @@
         <v>4</v>
       </c>
       <c r="F36" t="n">
-        <v>2</v>
+        <v>2.99622205531022</v>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
@@ -3584,7 +3584,7 @@
         <v>3</v>
       </c>
       <c r="F37" t="n">
-        <v>1.4</v>
+        <v>2.7</v>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
@@ -3668,7 +3668,7 @@
         <v>2</v>
       </c>
       <c r="F38" t="n">
-        <v>1.2</v>
+        <v>2.6</v>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
@@ -3752,7 +3752,7 @@
         <v>2</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
@@ -3836,7 +3836,7 @@
         <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
@@ -3920,7 +3920,7 @@
         <v>1</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
@@ -4004,7 +4004,7 @@
         <v>19</v>
       </c>
       <c r="F42" t="n">
-        <v>4.6</v>
+        <v>4.3</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -4092,7 +4092,7 @@
         <v>18</v>
       </c>
       <c r="F43" t="n">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
@@ -4176,7 +4176,7 @@
         <v>12</v>
       </c>
       <c r="F44" t="n">
-        <v>3</v>
+        <v>3.310260884226892</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -4264,7 +4264,7 @@
         <v>7</v>
       </c>
       <c r="F45" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
@@ -4348,7 +4348,7 @@
         <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -4436,7 +4436,7 @@
         <v>6</v>
       </c>
       <c r="F47" t="n">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
@@ -4520,7 +4520,7 @@
         <v>6</v>
       </c>
       <c r="F48" t="n">
-        <v>3</v>
+        <v>3.164444124696587</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -4608,7 +4608,7 @@
         <v>4</v>
       </c>
       <c r="F49" t="n">
-        <v>2.3</v>
+        <v>2.8</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -4696,7 +4696,7 @@
         <v>2</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>2.816175476572325</v>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
@@ -4780,7 +4780,7 @@
         <v>1</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>2.816175476572325</v>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
@@ -4864,7 +4864,7 @@
         <v>13</v>
       </c>
       <c r="F52" t="n">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
@@ -4948,7 +4948,7 @@
         <v>11</v>
       </c>
       <c r="F53" t="n">
-        <v>2</v>
+        <v>3.016586461874449</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -5036,7 +5036,7 @@
         <v>2</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>2.907838999115257</v>
       </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
@@ -5120,7 +5120,7 @@
         <v>8</v>
       </c>
       <c r="F55" t="n">
-        <v>2</v>
+        <v>3.25624803064939</v>
       </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
@@ -5204,7 +5204,7 @@
         <v>1</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
@@ -5288,7 +5288,7 @@
         <v>1</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
@@ -5372,7 +5372,7 @@
         <v>6</v>
       </c>
       <c r="F58" t="n">
-        <v>1.9</v>
+        <v>2.9</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
@@ -5456,7 +5456,7 @@
         <v>6</v>
       </c>
       <c r="F59" t="n">
-        <v>2</v>
+        <v>2.99622205531022</v>
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
@@ -5540,7 +5540,7 @@
         <v>6</v>
       </c>
       <c r="F60" t="n">
-        <v>2</v>
+        <v>3.109789330019855</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -5628,7 +5628,7 @@
         <v>6</v>
       </c>
       <c r="F61" t="n">
-        <v>2</v>
+        <v>2.99622205531022</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -5716,7 +5716,7 @@
         <v>5</v>
       </c>
       <c r="F62" t="n">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
@@ -5800,7 +5800,7 @@
         <v>5</v>
       </c>
       <c r="F63" t="n">
-        <v>1</v>
+        <v>2.957872047908649</v>
       </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="n">
@@ -5884,7 +5884,7 @@
         <v>5</v>
       </c>
       <c r="F64" t="n">
-        <v>2</v>
+        <v>2.99622205531022</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -5972,7 +5972,7 @@
         <v>3</v>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
@@ -6056,7 +6056,7 @@
         <v>3</v>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>2.840120762128931</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
@@ -6140,7 +6140,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="n">
@@ -6224,7 +6224,7 @@
         <v>8</v>
       </c>
       <c r="F68" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
@@ -6308,7 +6308,7 @@
         <v>8</v>
       </c>
       <c r="F69" t="n">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
@@ -6476,7 +6476,7 @@
         <v>5</v>
       </c>
       <c r="F71" t="n">
-        <v>2</v>
+        <v>3.038286869158483</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -6564,7 +6564,7 @@
         <v>5</v>
       </c>
       <c r="F72" t="n">
-        <v>2</v>
+        <v>2.951982378418139</v>
       </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="n">
@@ -6648,7 +6648,7 @@
         <v>4</v>
       </c>
       <c r="F73" t="n">
-        <v>1.6</v>
+        <v>2.6</v>
       </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="n">
@@ -6732,7 +6732,7 @@
         <v>3</v>
       </c>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -6820,7 +6820,7 @@
         <v>1</v>
       </c>
       <c r="F75" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
@@ -6988,7 +6988,7 @@
         <v>1</v>
       </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="n">
@@ -7156,7 +7156,7 @@
         <v>12</v>
       </c>
       <c r="F79" t="n">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -7244,7 +7244,7 @@
         <v>12</v>
       </c>
       <c r="F80" t="n">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -7332,7 +7332,7 @@
         <v>9</v>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>2.929030179863412</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -7420,7 +7420,7 @@
         <v>4</v>
       </c>
       <c r="F82" t="n">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -7508,7 +7508,7 @@
         <v>6</v>
       </c>
       <c r="F83" t="n">
-        <v>2</v>
+        <v>3.171923192807766</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -7596,7 +7596,7 @@
         <v>3</v>
       </c>
       <c r="F84" t="n">
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -7684,7 +7684,7 @@
         <v>1</v>
       </c>
       <c r="F85" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="n">
@@ -7768,7 +7768,7 @@
         <v>1</v>
       </c>
       <c r="F86" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="n">
@@ -7852,7 +7852,7 @@
         <v>10</v>
       </c>
       <c r="F87" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -7940,7 +7940,7 @@
         <v>8</v>
       </c>
       <c r="F88" t="n">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
         <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>1.9</v>
+        <v>2.8</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="n">
@@ -8112,7 +8112,7 @@
         <v>5</v>
       </c>
       <c r="F90" t="n">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -8200,7 +8200,7 @@
         <v>5</v>
       </c>
       <c r="F91" t="n">
-        <v>1.8</v>
+        <v>2.6</v>
       </c>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="n">
@@ -8284,7 +8284,7 @@
         <v>3</v>
       </c>
       <c r="F92" t="n">
-        <v>1.1</v>
+        <v>2.6</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -8372,7 +8372,7 @@
         <v>2</v>
       </c>
       <c r="F93" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="n">
@@ -8456,7 +8456,7 @@
         <v>2</v>
       </c>
       <c r="F94" t="n">
-        <v>2</v>
+        <v>3.034273399010271</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -8544,7 +8544,7 @@
         <v>1</v>
       </c>
       <c r="F95" t="n">
-        <v>1.2</v>
+        <v>2.4</v>
       </c>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="n">
@@ -8628,7 +8628,7 @@
         <v>1</v>
       </c>
       <c r="F96" t="n">
-        <v>1</v>
+        <v>2.799626141584827</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="n">
@@ -8712,7 +8712,7 @@
         <v>14</v>
       </c>
       <c r="F97" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="n">
@@ -8796,7 +8796,7 @@
         <v>8</v>
       </c>
       <c r="F98" t="n">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="G98" t="inlineStr"/>
       <c r="H98" t="n">
@@ -8880,7 +8880,7 @@
         <v>7</v>
       </c>
       <c r="F99" t="n">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="n">
@@ -8964,7 +8964,7 @@
         <v>5</v>
       </c>
       <c r="F100" t="n">
-        <v>1.1</v>
+        <v>2.6</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -9052,7 +9052,7 @@
         <v>5</v>
       </c>
       <c r="F101" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -9140,7 +9140,7 @@
         <v>4</v>
       </c>
       <c r="F102" t="n">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="n">
@@ -9224,7 +9224,7 @@
         <v>4</v>
       </c>
       <c r="F103" t="n">
-        <v>1.4</v>
+        <v>2.7</v>
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="n">
@@ -9308,7 +9308,7 @@
         <v>4</v>
       </c>
       <c r="F104" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -9480,7 +9480,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="n">
-        <v>1</v>
+        <v>2.839508134604157</v>
       </c>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="n">
@@ -9564,7 +9564,7 @@
         <v>14</v>
       </c>
       <c r="F107" t="n">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="n">
@@ -9648,7 +9648,7 @@
         <v>12</v>
       </c>
       <c r="F108" t="n">
-        <v>3.3</v>
+        <v>2.9</v>
       </c>
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="n">
@@ -9732,7 +9732,7 @@
         <v>5</v>
       </c>
       <c r="F109" t="n">
-        <v>1</v>
+        <v>2.923705019361567</v>
       </c>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="n">
@@ -9816,7 +9816,7 @@
         <v>2</v>
       </c>
       <c r="F110" t="n">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="n">
@@ -9900,7 +9900,7 @@
         <v>2</v>
       </c>
       <c r="F111" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="n">
@@ -9984,7 +9984,7 @@
         <v>1</v>
       </c>
       <c r="F112" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="n">
@@ -10068,7 +10068,7 @@
         <v>10</v>
       </c>
       <c r="F113" t="n">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -10156,7 +10156,7 @@
         <v>2</v>
       </c>
       <c r="F114" t="n">
-        <v>2</v>
+        <v>3.340367044251281</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -10244,7 +10244,7 @@
         <v>1</v>
       </c>
       <c r="F115" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="n">
@@ -10328,7 +10328,7 @@
         <v>11</v>
       </c>
       <c r="F116" t="n">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -10416,7 +10416,7 @@
         <v>10</v>
       </c>
       <c r="F117" t="n">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="n">
@@ -10500,7 +10500,7 @@
         <v>7</v>
       </c>
       <c r="F118" t="n">
-        <v>2.8</v>
+        <v>3.3</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -10588,7 +10588,7 @@
         <v>7</v>
       </c>
       <c r="F119" t="n">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="n">
@@ -10672,7 +10672,7 @@
         <v>7</v>
       </c>
       <c r="F120" t="n">
-        <v>3</v>
+        <v>3.184964454415507</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -10760,7 +10760,7 @@
         <v>5</v>
       </c>
       <c r="F121" t="n">
-        <v>1.7</v>
+        <v>2.7</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -10848,7 +10848,7 @@
         <v>5</v>
       </c>
       <c r="F122" t="n">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="n">
@@ -10932,7 +10932,7 @@
         <v>2</v>
       </c>
       <c r="F123" t="n">
-        <v>2</v>
+        <v>3.034273399010271</v>
       </c>
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="n">
@@ -11016,7 +11016,7 @@
         <v>1</v>
       </c>
       <c r="F124" t="n">
-        <v>1</v>
+        <v>2.799626141584827</v>
       </c>
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="n">
@@ -11100,7 +11100,7 @@
         <v>15</v>
       </c>
       <c r="F125" t="n">
-        <v>3.9</v>
+        <v>3.5</v>
       </c>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="n">
@@ -11184,7 +11184,7 @@
         <v>12</v>
       </c>
       <c r="F126" t="n">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="n">
@@ -11268,7 +11268,7 @@
         <v>11</v>
       </c>
       <c r="F127" t="n">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="G127" t="inlineStr"/>
       <c r="H127" t="n">
@@ -11352,7 +11352,7 @@
         <v>10</v>
       </c>
       <c r="F128" t="n">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -11440,7 +11440,7 @@
         <v>9</v>
       </c>
       <c r="F129" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="n">
@@ -11524,7 +11524,7 @@
         <v>8</v>
       </c>
       <c r="F130" t="n">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="n">
@@ -11608,7 +11608,7 @@
         <v>8</v>
       </c>
       <c r="F131" t="n">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="n">
@@ -11692,7 +11692,7 @@
         <v>8</v>
       </c>
       <c r="F132" t="n">
-        <v>1.9</v>
+        <v>2.8</v>
       </c>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="n">
@@ -11776,7 +11776,7 @@
         <v>7</v>
       </c>
       <c r="F133" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -11864,7 +11864,7 @@
         <v>6</v>
       </c>
       <c r="F134" t="n">
-        <v>2.3</v>
+        <v>2.8</v>
       </c>
       <c r="G134" t="inlineStr"/>
       <c r="H134" t="n">
@@ -11948,7 +11948,7 @@
         <v>4</v>
       </c>
       <c r="F135" t="n">
-        <v>2</v>
+        <v>2.995446630295157</v>
       </c>
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="n">
@@ -12032,7 +12032,7 @@
         <v>2</v>
       </c>
       <c r="F136" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G136" t="inlineStr"/>
       <c r="H136" t="n">
@@ -12204,7 +12204,7 @@
         <v>17</v>
       </c>
       <c r="F138" t="n">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="n">
@@ -12288,7 +12288,7 @@
         <v>15</v>
       </c>
       <c r="F139" t="n">
-        <v>3</v>
+        <v>3.227463491590079</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
@@ -12376,7 +12376,7 @@
         <v>11</v>
       </c>
       <c r="F140" t="n">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="G140" t="inlineStr"/>
       <c r="H140" t="n">
@@ -12460,7 +12460,7 @@
         <v>8</v>
       </c>
       <c r="F141" t="n">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="n">
@@ -12544,7 +12544,7 @@
         <v>5</v>
       </c>
       <c r="F142" t="n">
-        <v>1</v>
+        <v>3.115824763403007</v>
       </c>
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="n">
@@ -12628,7 +12628,7 @@
         <v>2</v>
       </c>
       <c r="F143" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G143" t="inlineStr"/>
       <c r="H143" t="n">
@@ -12712,7 +12712,7 @@
         <v>1</v>
       </c>
       <c r="F144" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G144" t="inlineStr"/>
       <c r="H144" t="n">
@@ -12796,7 +12796,7 @@
         <v>6</v>
       </c>
       <c r="F145" t="n">
-        <v>2.3</v>
+        <v>3</v>
       </c>
       <c r="G145" t="inlineStr"/>
       <c r="H145" t="n">
@@ -12880,7 +12880,7 @@
         <v>6</v>
       </c>
       <c r="F146" t="n">
-        <v>1.2</v>
+        <v>2.6</v>
       </c>
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="n">
@@ -12964,7 +12964,7 @@
         <v>5</v>
       </c>
       <c r="F147" t="n">
-        <v>1</v>
+        <v>2.957872047908649</v>
       </c>
       <c r="G147" t="inlineStr"/>
       <c r="H147" t="n">
@@ -13048,7 +13048,7 @@
         <v>3</v>
       </c>
       <c r="F148" t="n">
-        <v>1.9</v>
+        <v>2.9</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -13136,7 +13136,7 @@
         <v>2</v>
       </c>
       <c r="F149" t="n">
-        <v>2</v>
+        <v>3.034273399010271</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -13224,7 +13224,7 @@
         <v>1</v>
       </c>
       <c r="F150" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="n">
@@ -13308,7 +13308,7 @@
         <v>1</v>
       </c>
       <c r="F151" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="n">
@@ -13392,7 +13392,7 @@
         <v>1</v>
       </c>
       <c r="F152" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="n">
@@ -13476,7 +13476,7 @@
         <v>8</v>
       </c>
       <c r="F153" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="n">
@@ -13560,7 +13560,7 @@
         <v>8</v>
       </c>
       <c r="F154" t="n">
-        <v>3</v>
+        <v>3.164444124696587</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
@@ -13648,7 +13648,7 @@
         <v>6</v>
       </c>
       <c r="F155" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="n">
@@ -13732,7 +13732,7 @@
         <v>5</v>
       </c>
       <c r="F156" t="n">
-        <v>1</v>
+        <v>2.907734612648776</v>
       </c>
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="n">
@@ -13816,7 +13816,7 @@
         <v>4</v>
       </c>
       <c r="F157" t="n">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="n">
@@ -13900,7 +13900,7 @@
         <v>4</v>
       </c>
       <c r="F158" t="n">
-        <v>1</v>
+        <v>2.907734612648776</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
@@ -13988,7 +13988,7 @@
         <v>3</v>
       </c>
       <c r="F159" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="n">
@@ -14072,7 +14072,7 @@
         <v>3</v>
       </c>
       <c r="F160" t="n">
-        <v>1</v>
+        <v>2.907734612648776</v>
       </c>
       <c r="G160" t="inlineStr"/>
       <c r="H160" t="n">
@@ -14156,7 +14156,7 @@
         <v>3</v>
       </c>
       <c r="F161" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
@@ -14244,7 +14244,7 @@
         <v>1</v>
       </c>
       <c r="F162" t="n">
-        <v>1</v>
+        <v>2.839508134604157</v>
       </c>
       <c r="G162" t="inlineStr"/>
       <c r="H162" t="n">
@@ -14328,7 +14328,7 @@
         <v>10</v>
       </c>
       <c r="F163" t="n">
-        <v>2</v>
+        <v>3.033469806835996</v>
       </c>
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="n">
@@ -14412,7 +14412,7 @@
         <v>6</v>
       </c>
       <c r="F164" t="n">
-        <v>2</v>
+        <v>2.94511315530039</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -14500,7 +14500,7 @@
         <v>4</v>
       </c>
       <c r="F165" t="n">
-        <v>2</v>
+        <v>2.95592331196712</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -14588,7 +14588,7 @@
         <v>4</v>
       </c>
       <c r="F166" t="n">
-        <v>1</v>
+        <v>2.907838999115257</v>
       </c>
       <c r="G166" t="inlineStr"/>
       <c r="H166" t="n">
@@ -14672,7 +14672,7 @@
         <v>3</v>
       </c>
       <c r="F167" t="n">
-        <v>1</v>
+        <v>2.913109288464077</v>
       </c>
       <c r="G167" t="inlineStr"/>
       <c r="H167" t="n">
@@ -14756,7 +14756,7 @@
         <v>1</v>
       </c>
       <c r="F168" t="n">
-        <v>1</v>
+        <v>2.929030179863412</v>
       </c>
       <c r="G168" t="inlineStr"/>
       <c r="H168" t="n">
@@ -14840,7 +14840,7 @@
         <v>1</v>
       </c>
       <c r="F169" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="n">
@@ -14924,7 +14924,7 @@
         <v>8</v>
       </c>
       <c r="F170" t="n">
-        <v>2</v>
+        <v>3.368306191947591</v>
       </c>
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="n">
@@ -15008,7 +15008,7 @@
         <v>1</v>
       </c>
       <c r="F171" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="n">
@@ -15092,7 +15092,7 @@
         <v>1</v>
       </c>
       <c r="F172" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G172" t="inlineStr"/>
       <c r="H172" t="n">
@@ -15176,7 +15176,7 @@
         <v>8</v>
       </c>
       <c r="F173" t="n">
-        <v>3</v>
+        <v>3.184964454415507</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
@@ -15264,7 +15264,7 @@
         <v>6</v>
       </c>
       <c r="F174" t="n">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
       <c r="G174" t="inlineStr"/>
       <c r="H174" t="n">
@@ -15348,7 +15348,7 @@
         <v>6</v>
       </c>
       <c r="F175" t="n">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="n">
@@ -15432,7 +15432,7 @@
         <v>5</v>
       </c>
       <c r="F176" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -15520,7 +15520,7 @@
         <v>4</v>
       </c>
       <c r="F177" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="n">
@@ -15604,7 +15604,7 @@
         <v>4</v>
       </c>
       <c r="F178" t="n">
-        <v>1</v>
+        <v>2.879920376637045</v>
       </c>
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="n">
@@ -15688,7 +15688,7 @@
         <v>3</v>
       </c>
       <c r="F179" t="n">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
       <c r="G179" t="inlineStr"/>
       <c r="H179" t="n">
@@ -15772,7 +15772,7 @@
         <v>3</v>
       </c>
       <c r="F180" t="n">
-        <v>1</v>
+        <v>2.7</v>
       </c>
       <c r="G180" t="inlineStr"/>
       <c r="H180" t="n">
@@ -15856,7 +15856,7 @@
         <v>2</v>
       </c>
       <c r="F181" t="n">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="n">
@@ -15940,7 +15940,7 @@
         <v>2</v>
       </c>
       <c r="F182" t="n">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="n">
@@ -16024,7 +16024,7 @@
         <v>1</v>
       </c>
       <c r="F183" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G183" t="inlineStr"/>
       <c r="H183" t="n">
@@ -16108,7 +16108,7 @@
         <v>15</v>
       </c>
       <c r="F184" t="n">
-        <v>4.1</v>
+        <v>3.9</v>
       </c>
       <c r="G184" t="inlineStr"/>
       <c r="H184" t="n">
@@ -16192,7 +16192,7 @@
         <v>14</v>
       </c>
       <c r="F185" t="n">
-        <v>4</v>
+        <v>4.143103091798943</v>
       </c>
       <c r="G185" t="inlineStr"/>
       <c r="H185" t="n">
@@ -16276,7 +16276,7 @@
         <v>8</v>
       </c>
       <c r="F186" t="n">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
@@ -16364,7 +16364,7 @@
         <v>8</v>
       </c>
       <c r="F187" t="n">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="n">
@@ -16448,7 +16448,7 @@
         <v>7</v>
       </c>
       <c r="F188" t="n">
-        <v>2</v>
+        <v>3.059518858106242</v>
       </c>
       <c r="G188" t="inlineStr"/>
       <c r="H188" t="n">
@@ -16532,7 +16532,7 @@
         <v>6</v>
       </c>
       <c r="F189" t="n">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="G189" t="inlineStr"/>
       <c r="H189" t="n">
@@ -16616,7 +16616,7 @@
         <v>5</v>
       </c>
       <c r="F190" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -16704,7 +16704,7 @@
         <v>4</v>
       </c>
       <c r="F191" t="n">
-        <v>1</v>
+        <v>2.907734612648776</v>
       </c>
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="n">
@@ -16788,7 +16788,7 @@
         <v>2</v>
       </c>
       <c r="F192" t="n">
-        <v>1</v>
+        <v>2.885263000089072</v>
       </c>
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="n">
@@ -16872,7 +16872,7 @@
         <v>23</v>
       </c>
       <c r="F193" t="n">
-        <v>4</v>
+        <v>3.651846354220264</v>
       </c>
       <c r="G193" t="inlineStr"/>
       <c r="H193" t="n">
@@ -16956,7 +16956,7 @@
         <v>3</v>
       </c>
       <c r="F194" t="n">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="G194" t="inlineStr"/>
       <c r="H194" t="n">
@@ -17040,7 +17040,7 @@
         <v>1</v>
       </c>
       <c r="F195" t="n">
-        <v>1</v>
+        <v>2.892140121749447</v>
       </c>
       <c r="G195" t="inlineStr"/>
       <c r="H195" t="n">
@@ -17124,7 +17124,7 @@
         <v>1</v>
       </c>
       <c r="F196" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G196" t="inlineStr"/>
       <c r="H196" t="n">
@@ -17208,7 +17208,7 @@
         <v>16</v>
       </c>
       <c r="F197" t="n">
-        <v>5</v>
+        <v>4.753218168208356</v>
       </c>
       <c r="G197" t="inlineStr"/>
       <c r="H197" t="n">
@@ -17292,7 +17292,7 @@
         <v>1</v>
       </c>
       <c r="F198" t="n">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="G198" t="inlineStr"/>
       <c r="H198" t="n">
@@ -17376,7 +17376,7 @@
         <v>1</v>
       </c>
       <c r="F199" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G199" t="inlineStr"/>
       <c r="H199" t="n">
@@ -17548,7 +17548,7 @@
         <v>17</v>
       </c>
       <c r="F201" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
@@ -17636,7 +17636,7 @@
         <v>14</v>
       </c>
       <c r="F202" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="G202" t="inlineStr"/>
       <c r="H202" t="n">
@@ -17720,7 +17720,7 @@
         <v>14</v>
       </c>
       <c r="F203" t="n">
-        <v>4.1</v>
+        <v>4</v>
       </c>
       <c r="G203" t="inlineStr">
         <is>
@@ -17808,7 +17808,7 @@
         <v>14</v>
       </c>
       <c r="F204" t="n">
-        <v>5</v>
+        <v>4.566620097280829</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
@@ -17896,7 +17896,7 @@
         <v>12</v>
       </c>
       <c r="F205" t="n">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="G205" t="inlineStr">
         <is>
@@ -17984,7 +17984,7 @@
         <v>10</v>
       </c>
       <c r="F206" t="n">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
@@ -18072,7 +18072,7 @@
         <v>10</v>
       </c>
       <c r="F207" t="n">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="G207" t="inlineStr">
         <is>
@@ -18160,7 +18160,7 @@
         <v>8</v>
       </c>
       <c r="F208" t="n">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>
@@ -18248,7 +18248,7 @@
         <v>3</v>
       </c>
       <c r="F209" t="n">
-        <v>1</v>
+        <v>2.957872047908649</v>
       </c>
       <c r="G209" t="inlineStr"/>
       <c r="H209" t="n">
@@ -18332,7 +18332,7 @@
         <v>20</v>
       </c>
       <c r="F210" t="n">
-        <v>4.6</v>
+        <v>4</v>
       </c>
       <c r="G210" t="inlineStr"/>
       <c r="H210" t="n">
@@ -18416,7 +18416,7 @@
         <v>17</v>
       </c>
       <c r="F211" t="n">
-        <v>4.2</v>
+        <v>4.1</v>
       </c>
       <c r="G211" t="inlineStr"/>
       <c r="H211" t="n">
@@ -18500,7 +18500,7 @@
         <v>17</v>
       </c>
       <c r="F212" t="n">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="G212" t="inlineStr">
         <is>
@@ -18588,7 +18588,7 @@
         <v>13</v>
       </c>
       <c r="F213" t="n">
-        <v>4.2</v>
+        <v>3.8</v>
       </c>
       <c r="G213" t="inlineStr">
         <is>
@@ -18676,7 +18676,7 @@
         <v>9</v>
       </c>
       <c r="F214" t="n">
-        <v>3</v>
+        <v>3.164444124696587</v>
       </c>
       <c r="G214" t="inlineStr"/>
       <c r="H214" t="n">
@@ -18760,7 +18760,7 @@
         <v>6</v>
       </c>
       <c r="F215" t="n">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="G215" t="inlineStr"/>
       <c r="H215" t="n">
@@ -18844,7 +18844,7 @@
         <v>3</v>
       </c>
       <c r="F216" t="n">
-        <v>1.8</v>
+        <v>2.7</v>
       </c>
       <c r="G216" t="inlineStr"/>
       <c r="H216" t="n">
@@ -18928,7 +18928,7 @@
         <v>40</v>
       </c>
       <c r="F217" t="n">
-        <v>4.8</v>
+        <v>4.4</v>
       </c>
       <c r="G217" t="inlineStr"/>
       <c r="H217" t="n">
@@ -19012,7 +19012,7 @@
         <v>25</v>
       </c>
       <c r="F218" t="n">
-        <v>4</v>
+        <v>3.987374162437464</v>
       </c>
       <c r="G218" t="inlineStr">
         <is>
@@ -19188,7 +19188,7 @@
         <v>14</v>
       </c>
       <c r="F220" t="n">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="G220" t="inlineStr"/>
       <c r="H220" t="n">
@@ -19272,7 +19272,7 @@
         <v>15</v>
       </c>
       <c r="F221" t="n">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="G221" t="inlineStr"/>
       <c r="H221" t="n">
@@ -19356,7 +19356,7 @@
         <v>3</v>
       </c>
       <c r="F222" t="n">
-        <v>1.4</v>
+        <v>2.9</v>
       </c>
       <c r="G222" t="inlineStr"/>
       <c r="H222" t="n">
@@ -19440,7 +19440,7 @@
         <v>1</v>
       </c>
       <c r="F223" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G223" t="inlineStr"/>
       <c r="H223" t="n">
@@ -19608,7 +19608,7 @@
         <v>13</v>
       </c>
       <c r="F225" t="n">
-        <v>4.6</v>
+        <v>4.3</v>
       </c>
       <c r="G225" t="inlineStr"/>
       <c r="H225" t="n">
@@ -19780,7 +19780,7 @@
         <v>6</v>
       </c>
       <c r="F227" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="G227" t="inlineStr">
         <is>
@@ -19868,7 +19868,7 @@
         <v>6</v>
       </c>
       <c r="F228" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="G228" t="inlineStr">
         <is>
@@ -19956,7 +19956,7 @@
         <v>2</v>
       </c>
       <c r="F229" t="n">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="G229" t="inlineStr"/>
       <c r="H229" t="n">
@@ -20040,7 +20040,7 @@
         <v>2</v>
       </c>
       <c r="F230" t="n">
-        <v>1.9</v>
+        <v>3</v>
       </c>
       <c r="G230" t="inlineStr"/>
       <c r="H230" t="n">
@@ -20124,7 +20124,7 @@
         <v>1</v>
       </c>
       <c r="F231" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G231" t="inlineStr"/>
       <c r="H231" t="n">
@@ -20208,7 +20208,7 @@
         <v>22</v>
       </c>
       <c r="F232" t="n">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="G232" t="inlineStr"/>
       <c r="H232" t="n">
@@ -20292,7 +20292,7 @@
         <v>14</v>
       </c>
       <c r="F233" t="n">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="G233" t="inlineStr">
         <is>
@@ -20380,7 +20380,7 @@
         <v>12</v>
       </c>
       <c r="F234" t="n">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="G234" t="inlineStr">
         <is>
@@ -20468,7 +20468,7 @@
         <v>12</v>
       </c>
       <c r="F235" t="n">
-        <v>3</v>
+        <v>3.373116109750553</v>
       </c>
       <c r="G235" t="inlineStr">
         <is>
@@ -20556,7 +20556,7 @@
         <v>11</v>
       </c>
       <c r="F236" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="G236" t="inlineStr"/>
       <c r="H236" t="n">
@@ -20640,7 +20640,7 @@
         <v>10</v>
       </c>
       <c r="F237" t="n">
-        <v>3</v>
+        <v>3.457689272806166</v>
       </c>
       <c r="G237" t="inlineStr"/>
       <c r="H237" t="n">
@@ -20724,7 +20724,7 @@
         <v>8</v>
       </c>
       <c r="F238" t="n">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
       <c r="G238" t="inlineStr"/>
       <c r="H238" t="n">
@@ -20808,7 +20808,7 @@
         <v>5</v>
       </c>
       <c r="F239" t="n">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="G239" t="inlineStr"/>
       <c r="H239" t="n">
@@ -20892,7 +20892,7 @@
         <v>5</v>
       </c>
       <c r="F240" t="n">
-        <v>2</v>
+        <v>3.038286869158483</v>
       </c>
       <c r="G240" t="inlineStr"/>
       <c r="H240" t="n">
@@ -20976,7 +20976,7 @@
         <v>1</v>
       </c>
       <c r="F241" t="n">
-        <v>1</v>
+        <v>2.816175476572325</v>
       </c>
       <c r="G241" t="inlineStr"/>
       <c r="H241" t="n">
@@ -21060,7 +21060,7 @@
         <v>28</v>
       </c>
       <c r="F242" t="n">
-        <v>4.6</v>
+        <v>4.2</v>
       </c>
       <c r="G242" t="inlineStr">
         <is>
@@ -21148,7 +21148,7 @@
         <v>19</v>
       </c>
       <c r="F243" t="n">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="G243" t="inlineStr"/>
       <c r="H243" t="n">
@@ -21232,7 +21232,7 @@
         <v>18</v>
       </c>
       <c r="F244" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="G244" t="inlineStr">
         <is>
@@ -21404,7 +21404,7 @@
         <v>1</v>
       </c>
       <c r="F246" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G246" t="inlineStr"/>
       <c r="H246" t="n">
@@ -21488,7 +21488,7 @@
         <v>15</v>
       </c>
       <c r="F247" t="n">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="G247" t="inlineStr"/>
       <c r="H247" t="n">
@@ -21572,7 +21572,7 @@
         <v>1</v>
       </c>
       <c r="F248" t="n">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G248" t="inlineStr"/>
       <c r="H248" t="n">
@@ -21656,7 +21656,7 @@
         <v>1</v>
       </c>
       <c r="F249" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G249" t="inlineStr"/>
       <c r="H249" t="n">
@@ -21740,7 +21740,7 @@
         <v>13</v>
       </c>
       <c r="F250" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="G250" t="inlineStr"/>
       <c r="H250" t="n">
@@ -21824,7 +21824,7 @@
         <v>10</v>
       </c>
       <c r="F251" t="n">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="G251" t="inlineStr"/>
       <c r="H251" t="n">
@@ -21908,7 +21908,7 @@
         <v>7</v>
       </c>
       <c r="F252" t="n">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="G252" t="inlineStr">
         <is>
@@ -21996,7 +21996,7 @@
         <v>7</v>
       </c>
       <c r="F253" t="n">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="G253" t="inlineStr">
         <is>
@@ -22084,7 +22084,7 @@
         <v>6</v>
       </c>
       <c r="F254" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="G254" t="inlineStr">
         <is>
@@ -22172,7 +22172,7 @@
         <v>4</v>
       </c>
       <c r="F255" t="n">
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
       <c r="G255" t="inlineStr"/>
       <c r="H255" t="n">
@@ -22256,7 +22256,7 @@
         <v>4</v>
       </c>
       <c r="F256" t="n">
-        <v>2.2</v>
+        <v>3</v>
       </c>
       <c r="G256" t="inlineStr"/>
       <c r="H256" t="n">
@@ -22340,7 +22340,7 @@
         <v>1</v>
       </c>
       <c r="F257" t="n">
-        <v>1</v>
+        <v>2.799626141584827</v>
       </c>
       <c r="G257" t="inlineStr"/>
       <c r="H257" t="n">
@@ -22424,7 +22424,7 @@
         <v>26</v>
       </c>
       <c r="F258" t="n">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="G258" t="inlineStr"/>
       <c r="H258" t="n">
@@ -22508,7 +22508,7 @@
         <v>22</v>
       </c>
       <c r="F259" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="G259" t="inlineStr"/>
       <c r="H259" t="n">
@@ -22592,7 +22592,7 @@
         <v>22</v>
       </c>
       <c r="F260" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="G260" t="inlineStr">
         <is>
@@ -22680,7 +22680,7 @@
         <v>15</v>
       </c>
       <c r="F261" t="n">
-        <v>4</v>
+        <v>4.209338482842798</v>
       </c>
       <c r="G261" t="inlineStr">
         <is>
@@ -22768,7 +22768,7 @@
         <v>13</v>
       </c>
       <c r="F262" t="n">
-        <v>4</v>
+        <v>3.50037461706449</v>
       </c>
       <c r="G262" t="inlineStr">
         <is>
@@ -22856,7 +22856,7 @@
         <v>8</v>
       </c>
       <c r="F263" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="G263" t="inlineStr">
         <is>
@@ -22944,7 +22944,7 @@
         <v>6</v>
       </c>
       <c r="F264" t="n">
-        <v>2.3</v>
+        <v>2.8</v>
       </c>
       <c r="G264" t="inlineStr"/>
       <c r="H264" t="n">
@@ -23028,7 +23028,7 @@
         <v>4</v>
       </c>
       <c r="F265" t="n">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="G265" t="inlineStr">
         <is>
@@ -23116,7 +23116,7 @@
         <v>3</v>
       </c>
       <c r="F266" t="n">
-        <v>1.9</v>
+        <v>2.8</v>
       </c>
       <c r="G266" t="inlineStr"/>
       <c r="H266" t="n">
@@ -23200,7 +23200,7 @@
         <v>31</v>
       </c>
       <c r="F267" t="n">
-        <v>4.6</v>
+        <v>4.4</v>
       </c>
       <c r="G267" t="inlineStr"/>
       <c r="H267" t="n">
@@ -23284,7 +23284,7 @@
         <v>12</v>
       </c>
       <c r="F268" t="n">
-        <v>2</v>
+        <v>3.033469806835996</v>
       </c>
       <c r="G268" t="inlineStr"/>
       <c r="H268" t="n">
@@ -23368,7 +23368,7 @@
         <v>11</v>
       </c>
       <c r="F269" t="n">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="G269" t="inlineStr"/>
       <c r="H269" t="n">
@@ -23452,7 +23452,7 @@
         <v>11</v>
       </c>
       <c r="F270" t="n">
-        <v>2</v>
+        <v>2.994296644515754</v>
       </c>
       <c r="G270" t="inlineStr">
         <is>
@@ -23540,7 +23540,7 @@
         <v>9</v>
       </c>
       <c r="F271" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="G271" t="inlineStr"/>
       <c r="H271" t="n">
@@ -23624,7 +23624,7 @@
         <v>1</v>
       </c>
       <c r="F272" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G272" t="inlineStr"/>
       <c r="H272" t="n">
@@ -23708,7 +23708,7 @@
         <v>1</v>
       </c>
       <c r="F273" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G273" t="inlineStr"/>
       <c r="H273" t="n">
@@ -23792,7 +23792,7 @@
         <v>11</v>
       </c>
       <c r="F274" t="n">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="G274" t="inlineStr"/>
       <c r="H274" t="n">
@@ -23876,7 +23876,7 @@
         <v>6</v>
       </c>
       <c r="F275" t="n">
-        <v>1.4</v>
+        <v>2.7</v>
       </c>
       <c r="G275" t="inlineStr"/>
       <c r="H275" t="n">
@@ -23960,7 +23960,7 @@
         <v>6</v>
       </c>
       <c r="F276" t="n">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="G276" t="inlineStr">
         <is>
@@ -24048,7 +24048,7 @@
         <v>5</v>
       </c>
       <c r="F277" t="n">
-        <v>1</v>
+        <v>2.957872047908649</v>
       </c>
       <c r="G277" t="inlineStr"/>
       <c r="H277" t="n">
@@ -24132,7 +24132,7 @@
         <v>3</v>
       </c>
       <c r="F278" t="n">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="G278" t="inlineStr">
         <is>
@@ -24220,7 +24220,7 @@
         <v>3</v>
       </c>
       <c r="F279" t="n">
-        <v>2</v>
+        <v>3.034273399010271</v>
       </c>
       <c r="G279" t="inlineStr"/>
       <c r="H279" t="n">
@@ -24304,7 +24304,7 @@
         <v>3</v>
       </c>
       <c r="F280" t="n">
-        <v>1</v>
+        <v>2.91913645020728</v>
       </c>
       <c r="G280" t="inlineStr"/>
       <c r="H280" t="n">
@@ -24388,7 +24388,7 @@
         <v>1</v>
       </c>
       <c r="F281" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="G281" t="inlineStr"/>
       <c r="H281" t="n">
@@ -24472,7 +24472,7 @@
         <v>1</v>
       </c>
       <c r="F282" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G282" t="inlineStr"/>
       <c r="H282" t="n">
@@ -24556,7 +24556,7 @@
         <v>18</v>
       </c>
       <c r="F283" t="n">
-        <v>4.4</v>
+        <v>3.9</v>
       </c>
       <c r="G283" t="inlineStr"/>
       <c r="H283" t="n">
@@ -24640,7 +24640,7 @@
         <v>7</v>
       </c>
       <c r="F284" t="n">
-        <v>2</v>
+        <v>3.01693535314954</v>
       </c>
       <c r="G284" t="inlineStr"/>
       <c r="H284" t="n">
@@ -24724,7 +24724,7 @@
         <v>6</v>
       </c>
       <c r="F285" t="n">
-        <v>1.6</v>
+        <v>2.6</v>
       </c>
       <c r="G285" t="inlineStr"/>
       <c r="H285" t="n">
@@ -24808,7 +24808,7 @@
         <v>6</v>
       </c>
       <c r="F286" t="n">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="G286" t="inlineStr">
         <is>
@@ -24896,7 +24896,7 @@
         <v>6</v>
       </c>
       <c r="F287" t="n">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="G287" t="inlineStr"/>
       <c r="H287" t="n">
@@ -24980,7 +24980,7 @@
         <v>6</v>
       </c>
       <c r="F288" t="n">
-        <v>2</v>
+        <v>3.122661398011503</v>
       </c>
       <c r="G288" t="inlineStr"/>
       <c r="H288" t="n">
@@ -25064,7 +25064,7 @@
         <v>6</v>
       </c>
       <c r="F289" t="n">
-        <v>1</v>
+        <v>2.929966981198159</v>
       </c>
       <c r="G289" t="inlineStr">
         <is>
@@ -25152,7 +25152,7 @@
         <v>1</v>
       </c>
       <c r="F290" t="n">
-        <v>1</v>
+        <v>2.907734612648776</v>
       </c>
       <c r="G290" t="inlineStr"/>
       <c r="H290" t="n">
@@ -25236,7 +25236,7 @@
         <v>13</v>
       </c>
       <c r="F291" t="n">
-        <v>3</v>
+        <v>3.257997772959726</v>
       </c>
       <c r="G291" t="inlineStr"/>
       <c r="H291" t="n">
@@ -25320,7 +25320,7 @@
         <v>11</v>
       </c>
       <c r="F292" t="n">
-        <v>2</v>
+        <v>3.033469806835996</v>
       </c>
       <c r="G292" t="inlineStr">
         <is>
@@ -25408,7 +25408,7 @@
         <v>9</v>
       </c>
       <c r="F293" t="n">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="G293" t="inlineStr">
         <is>
@@ -25496,7 +25496,7 @@
         <v>7</v>
       </c>
       <c r="F294" t="n">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="G294" t="inlineStr"/>
       <c r="H294" t="n">
@@ -25580,7 +25580,7 @@
         <v>1</v>
       </c>
       <c r="F295" t="n">
-        <v>1</v>
+        <v>2.892140121749447</v>
       </c>
       <c r="G295" t="inlineStr"/>
       <c r="H295" t="n">
@@ -25664,7 +25664,7 @@
         <v>1</v>
       </c>
       <c r="F296" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G296" t="inlineStr"/>
       <c r="H296" t="n">
@@ -25748,7 +25748,7 @@
         <v>17</v>
       </c>
       <c r="F297" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="G297" t="inlineStr"/>
       <c r="H297" t="n">
@@ -25832,7 +25832,7 @@
         <v>1</v>
       </c>
       <c r="F298" t="n">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="G298" t="inlineStr"/>
       <c r="H298" t="n">
@@ -25916,7 +25916,7 @@
         <v>1</v>
       </c>
       <c r="F299" t="n">
-        <v>1.6</v>
+        <v>3</v>
       </c>
       <c r="G299" t="inlineStr"/>
       <c r="H299" t="n">
@@ -26000,7 +26000,7 @@
         <v>18</v>
       </c>
       <c r="F300" t="n">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="G300" t="inlineStr"/>
       <c r="H300" t="n">
@@ -26084,7 +26084,7 @@
         <v>13</v>
       </c>
       <c r="F301" t="n">
-        <v>3.7</v>
+        <v>3.9</v>
       </c>
       <c r="G301" t="inlineStr"/>
       <c r="H301" t="n">
@@ -26168,7 +26168,7 @@
         <v>11</v>
       </c>
       <c r="F302" t="n">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="G302" t="inlineStr">
         <is>
@@ -26256,7 +26256,7 @@
         <v>10</v>
       </c>
       <c r="F303" t="n">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="G303" t="inlineStr">
         <is>
@@ -26344,7 +26344,7 @@
         <v>7</v>
       </c>
       <c r="F304" t="n">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="G304" t="inlineStr">
         <is>
@@ -26432,7 +26432,7 @@
         <v>3</v>
       </c>
       <c r="F305" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="G305" t="inlineStr">
         <is>
@@ -26520,7 +26520,7 @@
         <v>2</v>
       </c>
       <c r="F306" t="n">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="G306" t="inlineStr"/>
       <c r="H306" t="n">
@@ -26604,7 +26604,7 @@
         <v>1</v>
       </c>
       <c r="F307" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G307" t="inlineStr"/>
       <c r="H307" t="n">
@@ -26688,7 +26688,7 @@
         <v>20</v>
       </c>
       <c r="F308" t="n">
-        <v>5</v>
+        <v>5.031135312202207</v>
       </c>
       <c r="G308" t="inlineStr">
         <is>
@@ -26776,7 +26776,7 @@
         <v>19</v>
       </c>
       <c r="F309" t="n">
-        <v>5</v>
+        <v>4.401694884232473</v>
       </c>
       <c r="G309" t="inlineStr">
         <is>
@@ -26864,7 +26864,7 @@
         <v>14</v>
       </c>
       <c r="F310" t="n">
-        <v>3</v>
+        <v>3.478996485805844</v>
       </c>
       <c r="G310" t="inlineStr"/>
       <c r="H310" t="n">
@@ -26948,7 +26948,7 @@
         <v>13</v>
       </c>
       <c r="F311" t="n">
-        <v>4</v>
+        <v>3.630185720717336</v>
       </c>
       <c r="G311" t="inlineStr"/>
       <c r="H311" t="n">
@@ -27032,7 +27032,7 @@
         <v>9</v>
       </c>
       <c r="F312" t="n">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="G312" t="inlineStr"/>
       <c r="H312" t="n">
@@ -27116,7 +27116,7 @@
         <v>9</v>
       </c>
       <c r="F313" t="n">
-        <v>3</v>
+        <v>3.164444124696587</v>
       </c>
       <c r="G313" t="inlineStr">
         <is>
@@ -27204,7 +27204,7 @@
         <v>7</v>
       </c>
       <c r="F314" t="n">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="G314" t="inlineStr">
         <is>
@@ -27292,7 +27292,7 @@
         <v>6</v>
       </c>
       <c r="F315" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="G315" t="inlineStr"/>
       <c r="H315" t="n">
@@ -27376,7 +27376,7 @@
         <v>3</v>
       </c>
       <c r="F316" t="n">
-        <v>2</v>
+        <v>2.951982378418139</v>
       </c>
       <c r="G316" t="inlineStr"/>
       <c r="H316" t="n">
@@ -27460,7 +27460,7 @@
         <v>1</v>
       </c>
       <c r="F317" t="n">
-        <v>1</v>
+        <v>2.839508134604157</v>
       </c>
       <c r="G317" t="inlineStr"/>
       <c r="H317" t="n">
@@ -27544,7 +27544,7 @@
         <v>32</v>
       </c>
       <c r="F318" t="n">
-        <v>4.6</v>
+        <v>4</v>
       </c>
       <c r="G318" t="inlineStr"/>
       <c r="H318" t="n">
@@ -27628,7 +27628,7 @@
         <v>28</v>
       </c>
       <c r="F319" t="n">
-        <v>4</v>
+        <v>3.7</v>
       </c>
       <c r="G319" t="inlineStr"/>
       <c r="H319" t="n">
@@ -27712,7 +27712,7 @@
         <v>16</v>
       </c>
       <c r="F320" t="n">
-        <v>3</v>
+        <v>3.173187822654838</v>
       </c>
       <c r="G320" t="inlineStr"/>
       <c r="H320" t="n">
@@ -27796,7 +27796,7 @@
         <v>13</v>
       </c>
       <c r="F321" t="n">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="G321" t="inlineStr"/>
       <c r="H321" t="n">
@@ -27880,7 +27880,7 @@
         <v>12</v>
       </c>
       <c r="F322" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="G322" t="inlineStr"/>
       <c r="H322" t="n">
@@ -27964,7 +27964,7 @@
         <v>1</v>
       </c>
       <c r="F323" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G323" t="inlineStr"/>
       <c r="H323" t="n">
@@ -28048,7 +28048,7 @@
         <v>1</v>
       </c>
       <c r="F324" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G324" t="inlineStr"/>
       <c r="H324" t="n">
@@ -28132,7 +28132,7 @@
         <v>1</v>
       </c>
       <c r="F325" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G325" t="inlineStr"/>
       <c r="H325" t="n">
@@ -28216,7 +28216,7 @@
         <v>8</v>
       </c>
       <c r="F326" t="n">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="G326" t="inlineStr">
         <is>
@@ -28304,7 +28304,7 @@
         <v>8</v>
       </c>
       <c r="F327" t="n">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="G327" t="inlineStr"/>
       <c r="H327" t="n">
@@ -28388,7 +28388,7 @@
         <v>7</v>
       </c>
       <c r="F328" t="n">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="G328" t="inlineStr"/>
       <c r="H328" t="n">
@@ -28472,7 +28472,7 @@
         <v>7</v>
       </c>
       <c r="F329" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="G329" t="inlineStr">
         <is>
@@ -28560,7 +28560,7 @@
         <v>7</v>
       </c>
       <c r="F330" t="n">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="G330" t="inlineStr">
         <is>
@@ -28648,7 +28648,7 @@
         <v>6</v>
       </c>
       <c r="F331" t="n">
-        <v>1</v>
+        <v>2.7</v>
       </c>
       <c r="G331" t="inlineStr">
         <is>
@@ -28736,7 +28736,7 @@
         <v>3</v>
       </c>
       <c r="F332" t="n">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="G332" t="inlineStr"/>
       <c r="H332" t="n">
@@ -28820,7 +28820,7 @@
         <v>2</v>
       </c>
       <c r="F333" t="n">
-        <v>1</v>
+        <v>2.879920376637045</v>
       </c>
       <c r="G333" t="inlineStr"/>
       <c r="H333" t="n">
@@ -28904,7 +28904,7 @@
         <v>1</v>
       </c>
       <c r="F334" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G334" t="inlineStr"/>
       <c r="H334" t="n">
@@ -28988,7 +28988,7 @@
         <v>1</v>
       </c>
       <c r="F335" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G335" t="inlineStr"/>
       <c r="H335" t="n">
@@ -29072,7 +29072,7 @@
         <v>1</v>
       </c>
       <c r="F336" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G336" t="inlineStr"/>
       <c r="H336" t="n">
@@ -29156,7 +29156,7 @@
         <v>14</v>
       </c>
       <c r="F337" t="n">
-        <v>4</v>
+        <v>3.7</v>
       </c>
       <c r="G337" t="inlineStr"/>
       <c r="H337" t="n">
@@ -29240,7 +29240,7 @@
         <v>13</v>
       </c>
       <c r="F338" t="n">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="G338" t="inlineStr"/>
       <c r="H338" t="n">
@@ -29324,7 +29324,7 @@
         <v>12</v>
       </c>
       <c r="F339" t="n">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="G339" t="inlineStr"/>
       <c r="H339" t="n">
@@ -29408,7 +29408,7 @@
         <v>7</v>
       </c>
       <c r="F340" t="n">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="G340" t="inlineStr"/>
       <c r="H340" t="n">
@@ -29492,7 +29492,7 @@
         <v>6</v>
       </c>
       <c r="F341" t="n">
-        <v>1.6</v>
+        <v>2.6</v>
       </c>
       <c r="G341" t="inlineStr"/>
       <c r="H341" t="n">
@@ -29576,7 +29576,7 @@
         <v>2</v>
       </c>
       <c r="F342" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G342" t="inlineStr"/>
       <c r="H342" t="n">
@@ -29660,7 +29660,7 @@
         <v>2</v>
       </c>
       <c r="F343" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G343" t="inlineStr"/>
       <c r="H343" t="n">
@@ -29744,7 +29744,7 @@
         <v>1</v>
       </c>
       <c r="F344" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G344" t="inlineStr"/>
       <c r="H344" t="n">
@@ -29828,7 +29828,7 @@
         <v>1</v>
       </c>
       <c r="F345" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G345" t="inlineStr"/>
       <c r="H345" t="n">
@@ -29996,7 +29996,7 @@
         <v>10</v>
       </c>
       <c r="F347" t="n">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="G347" t="inlineStr">
         <is>
@@ -30084,7 +30084,7 @@
         <v>9</v>
       </c>
       <c r="F348" t="n">
-        <v>2.3</v>
+        <v>2.7</v>
       </c>
       <c r="G348" t="inlineStr">
         <is>
@@ -30172,7 +30172,7 @@
         <v>2</v>
       </c>
       <c r="F349" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G349" t="inlineStr"/>
       <c r="H349" t="n">
@@ -30256,7 +30256,7 @@
         <v>16</v>
       </c>
       <c r="F350" t="n">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="G350" t="inlineStr"/>
       <c r="H350" t="n">
@@ -30340,7 +30340,7 @@
         <v>1</v>
       </c>
       <c r="F351" t="n">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="G351" t="inlineStr"/>
       <c r="H351" t="n">
@@ -30424,7 +30424,7 @@
         <v>1</v>
       </c>
       <c r="F352" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G352" t="inlineStr"/>
       <c r="H352" t="n">
@@ -30676,7 +30676,7 @@
         <v>10</v>
       </c>
       <c r="F355" t="n">
-        <v>2.9</v>
+        <v>3.3</v>
       </c>
       <c r="G355" t="inlineStr">
         <is>
@@ -30764,7 +30764,7 @@
         <v>8</v>
       </c>
       <c r="F356" t="n">
-        <v>3</v>
+        <v>3.373982644933322</v>
       </c>
       <c r="G356" t="inlineStr">
         <is>
@@ -30852,7 +30852,7 @@
         <v>7</v>
       </c>
       <c r="F357" t="n">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="G357" t="inlineStr">
         <is>
@@ -30940,7 +30940,7 @@
         <v>6</v>
       </c>
       <c r="F358" t="n">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="G358" t="inlineStr">
         <is>
@@ -31028,7 +31028,7 @@
         <v>3</v>
       </c>
       <c r="F359" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="G359" t="inlineStr"/>
       <c r="H359" t="n">
@@ -31112,7 +31112,7 @@
         <v>3</v>
       </c>
       <c r="F360" t="n">
-        <v>1.4</v>
+        <v>2.5</v>
       </c>
       <c r="G360" t="inlineStr"/>
       <c r="H360" t="n">
@@ -31196,7 +31196,7 @@
         <v>21</v>
       </c>
       <c r="F361" t="n">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
       <c r="G361" t="inlineStr">
         <is>
@@ -31284,7 +31284,7 @@
         <v>15</v>
       </c>
       <c r="F362" t="n">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="G362" t="inlineStr">
         <is>
@@ -31372,7 +31372,7 @@
         <v>15</v>
       </c>
       <c r="F363" t="n">
-        <v>4</v>
+        <v>4.076239996037482</v>
       </c>
       <c r="G363" t="inlineStr">
         <is>
@@ -31460,7 +31460,7 @@
         <v>14</v>
       </c>
       <c r="F364" t="n">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="G364" t="inlineStr">
         <is>
@@ -31548,7 +31548,7 @@
         <v>14</v>
       </c>
       <c r="F365" t="n">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="G365" t="inlineStr"/>
       <c r="H365" t="n">
@@ -31632,7 +31632,7 @@
         <v>13</v>
       </c>
       <c r="F366" t="n">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="G366" t="inlineStr"/>
       <c r="H366" t="n">
@@ -31716,7 +31716,7 @@
         <v>6</v>
       </c>
       <c r="F367" t="n">
-        <v>2</v>
+        <v>3.038286869158483</v>
       </c>
       <c r="G367" t="inlineStr"/>
       <c r="H367" t="n">
@@ -31800,7 +31800,7 @@
         <v>2</v>
       </c>
       <c r="F368" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G368" t="inlineStr"/>
       <c r="H368" t="n">
@@ -31884,7 +31884,7 @@
         <v>1</v>
       </c>
       <c r="F369" t="n">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="G369" t="inlineStr"/>
       <c r="H369" t="n">
@@ -31968,7 +31968,7 @@
         <v>1</v>
       </c>
       <c r="F370" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G370" t="inlineStr"/>
       <c r="H370" t="n">
@@ -32052,7 +32052,7 @@
         <v>44</v>
       </c>
       <c r="F371" t="n">
-        <v>4.9</v>
+        <v>4.6</v>
       </c>
       <c r="G371" t="inlineStr"/>
       <c r="H371" t="n">
@@ -32136,7 +32136,7 @@
         <v>30</v>
       </c>
       <c r="F372" t="n">
-        <v>4.6</v>
+        <v>4.1</v>
       </c>
       <c r="G372" t="inlineStr"/>
       <c r="H372" t="n">
@@ -32304,7 +32304,7 @@
         <v>9</v>
       </c>
       <c r="F374" t="n">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="G374" t="inlineStr">
         <is>
@@ -32392,7 +32392,7 @@
         <v>12</v>
       </c>
       <c r="F375" t="n">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="G375" t="inlineStr"/>
       <c r="H375" t="n">
@@ -32476,7 +32476,7 @@
         <v>1</v>
       </c>
       <c r="F376" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G376" t="inlineStr"/>
       <c r="H376" t="n">
@@ -32560,7 +32560,7 @@
         <v>1</v>
       </c>
       <c r="F377" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G377" t="inlineStr"/>
       <c r="H377" t="n">
@@ -32644,7 +32644,7 @@
         <v>14</v>
       </c>
       <c r="F378" t="n">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
       <c r="G378" t="inlineStr"/>
       <c r="H378" t="n">
@@ -32728,7 +32728,7 @@
         <v>12</v>
       </c>
       <c r="F379" t="n">
-        <v>4.2</v>
+        <v>3.7</v>
       </c>
       <c r="G379" t="inlineStr">
         <is>
@@ -32816,7 +32816,7 @@
         <v>10</v>
       </c>
       <c r="F380" t="n">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="G380" t="inlineStr"/>
       <c r="H380" t="n">
@@ -32900,7 +32900,7 @@
         <v>8</v>
       </c>
       <c r="F381" t="n">
-        <v>3</v>
+        <v>3.412235019292254</v>
       </c>
       <c r="G381" t="inlineStr">
         <is>
@@ -32988,7 +32988,7 @@
         <v>8</v>
       </c>
       <c r="F382" t="n">
-        <v>2</v>
+        <v>3.109789330019855</v>
       </c>
       <c r="G382" t="inlineStr">
         <is>
@@ -33076,7 +33076,7 @@
         <v>6</v>
       </c>
       <c r="F383" t="n">
-        <v>3</v>
+        <v>3.373982644933322</v>
       </c>
       <c r="G383" t="inlineStr">
         <is>
@@ -33164,7 +33164,7 @@
         <v>3</v>
       </c>
       <c r="F384" t="n">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="G384" t="inlineStr"/>
       <c r="H384" t="n">
@@ -33248,7 +33248,7 @@
         <v>2</v>
       </c>
       <c r="F385" t="n">
-        <v>1.4</v>
+        <v>2.7</v>
       </c>
       <c r="G385" t="inlineStr"/>
       <c r="H385" t="n">
@@ -33332,7 +33332,7 @@
         <v>2</v>
       </c>
       <c r="F386" t="n">
-        <v>1.4</v>
+        <v>2.7</v>
       </c>
       <c r="G386" t="inlineStr"/>
       <c r="H386" t="n">
@@ -33416,7 +33416,7 @@
         <v>16</v>
       </c>
       <c r="F387" t="n">
-        <v>4.2</v>
+        <v>3.7</v>
       </c>
       <c r="G387" t="inlineStr">
         <is>
@@ -33504,7 +33504,7 @@
         <v>16</v>
       </c>
       <c r="F388" t="n">
-        <v>4</v>
+        <v>3.784758718396382</v>
       </c>
       <c r="G388" t="inlineStr">
         <is>
@@ -33592,7 +33592,7 @@
         <v>15</v>
       </c>
       <c r="F389" t="n">
-        <v>4.1</v>
+        <v>3.8</v>
       </c>
       <c r="G389" t="inlineStr"/>
       <c r="H389" t="n">
@@ -33676,7 +33676,7 @@
         <v>12</v>
       </c>
       <c r="F390" t="n">
-        <v>3</v>
+        <v>3.457689272806166</v>
       </c>
       <c r="G390" t="inlineStr">
         <is>
@@ -33764,7 +33764,7 @@
         <v>10</v>
       </c>
       <c r="F391" t="n">
-        <v>1.6</v>
+        <v>2.7</v>
       </c>
       <c r="G391" t="inlineStr">
         <is>
@@ -33852,7 +33852,7 @@
         <v>8</v>
       </c>
       <c r="F392" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="G392" t="inlineStr">
         <is>
@@ -33940,7 +33940,7 @@
         <v>7</v>
       </c>
       <c r="F393" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G393" t="inlineStr">
         <is>
@@ -34028,7 +34028,7 @@
         <v>6</v>
       </c>
       <c r="F394" t="n">
-        <v>2.3</v>
+        <v>2.8</v>
       </c>
       <c r="G394" t="inlineStr"/>
       <c r="H394" t="n">
@@ -34112,7 +34112,7 @@
         <v>1</v>
       </c>
       <c r="F395" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G395" t="inlineStr"/>
       <c r="H395" t="n">
@@ -34196,7 +34196,7 @@
         <v>30</v>
       </c>
       <c r="F396" t="n">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="G396" t="inlineStr"/>
       <c r="H396" t="n">
@@ -34280,7 +34280,7 @@
         <v>28</v>
       </c>
       <c r="F397" t="n">
-        <v>4.6</v>
+        <v>4</v>
       </c>
       <c r="G397" t="inlineStr"/>
       <c r="H397" t="n">
@@ -34364,7 +34364,7 @@
         <v>14</v>
       </c>
       <c r="F398" t="n">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="G398" t="inlineStr"/>
       <c r="H398" t="n">
@@ -34532,7 +34532,7 @@
         <v>12</v>
       </c>
       <c r="F400" t="n">
-        <v>3</v>
+        <v>3.102345790701446</v>
       </c>
       <c r="G400" t="inlineStr"/>
       <c r="H400" t="n">
@@ -34616,7 +34616,7 @@
         <v>9</v>
       </c>
       <c r="F401" t="n">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="G401" t="inlineStr"/>
       <c r="H401" t="n">
@@ -34700,7 +34700,7 @@
         <v>1</v>
       </c>
       <c r="F402" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G402" t="inlineStr"/>
       <c r="H402" t="n">
@@ -34784,7 +34784,7 @@
         <v>1</v>
       </c>
       <c r="F403" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G403" t="inlineStr"/>
       <c r="H403" t="n">
@@ -34868,7 +34868,7 @@
         <v>11</v>
       </c>
       <c r="F404" t="n">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="G404" t="inlineStr"/>
       <c r="H404" t="n">
@@ -34952,7 +34952,7 @@
         <v>7</v>
       </c>
       <c r="F405" t="n">
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
       <c r="G405" t="inlineStr">
         <is>
@@ -35040,7 +35040,7 @@
         <v>6</v>
       </c>
       <c r="F406" t="n">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G406" t="inlineStr"/>
       <c r="H406" t="n">
@@ -35124,7 +35124,7 @@
         <v>5</v>
       </c>
       <c r="F407" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G407" t="inlineStr"/>
       <c r="H407" t="n">
@@ -35208,7 +35208,7 @@
         <v>5</v>
       </c>
       <c r="F408" t="n">
-        <v>1.3</v>
+        <v>2.7</v>
       </c>
       <c r="G408" t="inlineStr"/>
       <c r="H408" t="n">
@@ -35292,7 +35292,7 @@
         <v>3</v>
       </c>
       <c r="F409" t="n">
-        <v>1.6</v>
+        <v>2.9</v>
       </c>
       <c r="G409" t="inlineStr"/>
       <c r="H409" t="n">
@@ -35376,7 +35376,7 @@
         <v>2</v>
       </c>
       <c r="F410" t="n">
-        <v>1.2</v>
+        <v>2.7</v>
       </c>
       <c r="G410" t="inlineStr"/>
       <c r="H410" t="n">
@@ -35460,7 +35460,7 @@
         <v>2</v>
       </c>
       <c r="F411" t="n">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="G411" t="inlineStr"/>
       <c r="H411" t="n">
@@ -35544,7 +35544,7 @@
         <v>1</v>
       </c>
       <c r="F412" t="n">
-        <v>1</v>
+        <v>2.3</v>
       </c>
       <c r="G412" t="inlineStr"/>
       <c r="H412" t="n">
@@ -35628,7 +35628,7 @@
         <v>17</v>
       </c>
       <c r="F413" t="n">
-        <v>4.7</v>
+        <v>4.1</v>
       </c>
       <c r="G413" t="inlineStr"/>
       <c r="H413" t="n">
@@ -35712,7 +35712,7 @@
         <v>8</v>
       </c>
       <c r="F414" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="G414" t="inlineStr"/>
       <c r="H414" t="n">
@@ -35796,7 +35796,7 @@
         <v>7</v>
       </c>
       <c r="F415" t="n">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="G415" t="inlineStr">
         <is>
@@ -35884,7 +35884,7 @@
         <v>5</v>
       </c>
       <c r="F416" t="n">
-        <v>1</v>
+        <v>2.907734612648776</v>
       </c>
       <c r="G416" t="inlineStr">
         <is>
@@ -35972,7 +35972,7 @@
         <v>4</v>
       </c>
       <c r="F417" t="n">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="G417" t="inlineStr"/>
       <c r="H417" t="n">
@@ -36056,7 +36056,7 @@
         <v>3</v>
       </c>
       <c r="F418" t="n">
-        <v>1.6</v>
+        <v>2.7</v>
       </c>
       <c r="G418" t="inlineStr"/>
       <c r="H418" t="n">
@@ -36140,7 +36140,7 @@
         <v>3</v>
       </c>
       <c r="F419" t="n">
-        <v>1</v>
+        <v>2.885263000089072</v>
       </c>
       <c r="G419" t="inlineStr"/>
       <c r="H419" t="n">
@@ -36224,7 +36224,7 @@
         <v>1</v>
       </c>
       <c r="F420" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G420" t="inlineStr"/>
       <c r="H420" t="n">
@@ -36308,7 +36308,7 @@
         <v>26</v>
       </c>
       <c r="F421" t="n">
-        <v>4.6</v>
+        <v>3.7</v>
       </c>
       <c r="G421" t="inlineStr"/>
       <c r="H421" t="n">
@@ -36392,7 +36392,7 @@
         <v>7</v>
       </c>
       <c r="F422" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G422" t="inlineStr">
         <is>
@@ -36480,7 +36480,7 @@
         <v>5</v>
       </c>
       <c r="F423" t="n">
-        <v>1</v>
+        <v>2.923705019361567</v>
       </c>
       <c r="G423" t="inlineStr"/>
       <c r="H423" t="n">
@@ -36564,7 +36564,7 @@
         <v>2</v>
       </c>
       <c r="F424" t="n">
-        <v>1</v>
+        <v>2.892140121749447</v>
       </c>
       <c r="G424" t="inlineStr"/>
       <c r="H424" t="n">
@@ -36648,7 +36648,7 @@
         <v>1</v>
       </c>
       <c r="F425" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G425" t="inlineStr"/>
       <c r="H425" t="n">
@@ -36732,7 +36732,7 @@
         <v>1</v>
       </c>
       <c r="F426" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G426" t="inlineStr"/>
       <c r="H426" t="n">
@@ -36816,7 +36816,7 @@
         <v>5</v>
       </c>
       <c r="F427" t="n">
-        <v>1.7</v>
+        <v>3</v>
       </c>
       <c r="G427" t="inlineStr"/>
       <c r="H427" t="n">
@@ -36900,7 +36900,7 @@
         <v>3</v>
       </c>
       <c r="F428" t="n">
-        <v>1.9</v>
+        <v>3.1</v>
       </c>
       <c r="G428" t="inlineStr"/>
       <c r="H428" t="n">
@@ -36984,7 +36984,7 @@
         <v>1</v>
       </c>
       <c r="F429" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G429" t="inlineStr"/>
       <c r="H429" t="n">
@@ -37068,7 +37068,7 @@
         <v>7</v>
       </c>
       <c r="F430" t="n">
-        <v>2</v>
+        <v>3.109789330019855</v>
       </c>
       <c r="G430" t="inlineStr">
         <is>
@@ -37156,7 +37156,7 @@
         <v>6</v>
       </c>
       <c r="F431" t="n">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
       <c r="G431" t="inlineStr">
         <is>
@@ -37244,7 +37244,7 @@
         <v>6</v>
       </c>
       <c r="F432" t="n">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="G432" t="inlineStr"/>
       <c r="H432" t="n">
@@ -37328,7 +37328,7 @@
         <v>6</v>
       </c>
       <c r="F433" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G433" t="inlineStr">
         <is>
@@ -37416,7 +37416,7 @@
         <v>5</v>
       </c>
       <c r="F434" t="n">
-        <v>1.4</v>
+        <v>2.2</v>
       </c>
       <c r="G434" t="inlineStr">
         <is>
@@ -37504,7 +37504,7 @@
         <v>4</v>
       </c>
       <c r="F435" t="n">
-        <v>1</v>
+        <v>2.7</v>
       </c>
       <c r="G435" t="inlineStr"/>
       <c r="H435" t="n">
@@ -37588,7 +37588,7 @@
         <v>3</v>
       </c>
       <c r="F436" t="n">
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="G436" t="inlineStr"/>
       <c r="H436" t="n">
@@ -37672,7 +37672,7 @@
         <v>2</v>
       </c>
       <c r="F437" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G437" t="inlineStr"/>
       <c r="H437" t="n">
@@ -37756,7 +37756,7 @@
         <v>13</v>
       </c>
       <c r="F438" t="n">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="G438" t="inlineStr">
         <is>
@@ -37844,7 +37844,7 @@
         <v>9</v>
       </c>
       <c r="F439" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="G439" t="inlineStr"/>
       <c r="H439" t="n">
@@ -37928,7 +37928,7 @@
         <v>6</v>
       </c>
       <c r="F440" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="G440" t="inlineStr">
         <is>
@@ -38016,7 +38016,7 @@
         <v>5</v>
       </c>
       <c r="F441" t="n">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="G441" t="inlineStr"/>
       <c r="H441" t="n">
@@ -38100,7 +38100,7 @@
         <v>5</v>
       </c>
       <c r="F442" t="n">
-        <v>2</v>
+        <v>3.038286869158483</v>
       </c>
       <c r="G442" t="inlineStr"/>
       <c r="H442" t="n">
@@ -38184,7 +38184,7 @@
         <v>4</v>
       </c>
       <c r="F443" t="n">
-        <v>2</v>
+        <v>2.951982378418139</v>
       </c>
       <c r="G443" t="inlineStr"/>
       <c r="H443" t="n">
@@ -38268,7 +38268,7 @@
         <v>2</v>
       </c>
       <c r="F444" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G444" t="inlineStr"/>
       <c r="H444" t="n">
@@ -38352,7 +38352,7 @@
         <v>2</v>
       </c>
       <c r="F445" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G445" t="inlineStr"/>
       <c r="H445" t="n">
@@ -38436,7 +38436,7 @@
         <v>1</v>
       </c>
       <c r="F446" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G446" t="inlineStr"/>
       <c r="H446" t="n">
@@ -38520,7 +38520,7 @@
         <v>30</v>
       </c>
       <c r="F447" t="n">
-        <v>4.6</v>
+        <v>4.2</v>
       </c>
       <c r="G447" t="inlineStr"/>
       <c r="H447" t="n">
@@ -38604,7 +38604,7 @@
         <v>21</v>
       </c>
       <c r="F448" t="n">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="G448" t="inlineStr"/>
       <c r="H448" t="n">
@@ -38688,7 +38688,7 @@
         <v>13</v>
       </c>
       <c r="F449" t="n">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="G449" t="inlineStr">
         <is>
@@ -38776,7 +38776,7 @@
         <v>11</v>
       </c>
       <c r="F450" t="n">
-        <v>2</v>
+        <v>2.999844965579115</v>
       </c>
       <c r="G450" t="inlineStr">
         <is>
@@ -38864,7 +38864,7 @@
         <v>9</v>
       </c>
       <c r="F451" t="n">
-        <v>1.8</v>
+        <v>2.6</v>
       </c>
       <c r="G451" t="inlineStr"/>
       <c r="H451" t="n">
@@ -38948,7 +38948,7 @@
         <v>4</v>
       </c>
       <c r="F452" t="n">
-        <v>1</v>
+        <v>2.907838999115257</v>
       </c>
       <c r="G452" t="inlineStr"/>
       <c r="H452" t="n">
@@ -39032,7 +39032,7 @@
         <v>2</v>
       </c>
       <c r="F453" t="n">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="G453" t="inlineStr"/>
       <c r="H453" t="n">
@@ -39116,7 +39116,7 @@
         <v>10</v>
       </c>
       <c r="F454" t="n">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
       <c r="G454" t="inlineStr"/>
       <c r="H454" t="n">
@@ -39200,7 +39200,7 @@
         <v>1</v>
       </c>
       <c r="F455" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G455" t="inlineStr"/>
       <c r="H455" t="n">
@@ -39284,7 +39284,7 @@
         <v>1</v>
       </c>
       <c r="F456" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G456" t="inlineStr"/>
       <c r="H456" t="n">
@@ -39368,7 +39368,7 @@
         <v>15</v>
       </c>
       <c r="F457" t="n">
-        <v>4.4</v>
+        <v>4</v>
       </c>
       <c r="G457" t="inlineStr"/>
       <c r="H457" t="n">
@@ -39452,7 +39452,7 @@
         <v>10</v>
       </c>
       <c r="F458" t="n">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="G458" t="inlineStr"/>
       <c r="H458" t="n">
@@ -39536,7 +39536,7 @@
         <v>8</v>
       </c>
       <c r="F459" t="n">
-        <v>1.9</v>
+        <v>2.9</v>
       </c>
       <c r="G459" t="inlineStr"/>
       <c r="H459" t="n">
@@ -39620,7 +39620,7 @@
         <v>7</v>
       </c>
       <c r="F460" t="n">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
       <c r="G460" t="inlineStr"/>
       <c r="H460" t="n">
@@ -39704,7 +39704,7 @@
         <v>6</v>
       </c>
       <c r="F461" t="n">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="G461" t="inlineStr"/>
       <c r="H461" t="n">
@@ -39788,7 +39788,7 @@
         <v>5</v>
       </c>
       <c r="F462" t="n">
-        <v>1.6</v>
+        <v>2.7</v>
       </c>
       <c r="G462" t="inlineStr"/>
       <c r="H462" t="n">
@@ -39872,7 +39872,7 @@
         <v>4</v>
       </c>
       <c r="F463" t="n">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="G463" t="inlineStr"/>
       <c r="H463" t="n">
@@ -39956,7 +39956,7 @@
         <v>3</v>
       </c>
       <c r="F464" t="n">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
       <c r="G464" t="inlineStr"/>
       <c r="H464" t="n">
@@ -40040,7 +40040,7 @@
         <v>3</v>
       </c>
       <c r="F465" t="n">
-        <v>1</v>
+        <v>2.879920376637045</v>
       </c>
       <c r="G465" t="inlineStr"/>
       <c r="H465" t="n">
@@ -40124,7 +40124,7 @@
         <v>1</v>
       </c>
       <c r="F466" t="n">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
       <c r="G466" t="inlineStr"/>
       <c r="H466" t="n">
@@ -40208,7 +40208,7 @@
         <v>1</v>
       </c>
       <c r="F467" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G467" t="inlineStr"/>
       <c r="H467" t="n">
@@ -40376,7 +40376,7 @@
         <v>13</v>
       </c>
       <c r="F469" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="G469" t="inlineStr"/>
       <c r="H469" t="n">
@@ -40460,7 +40460,7 @@
         <v>12</v>
       </c>
       <c r="F470" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="G470" t="inlineStr">
         <is>
@@ -40548,7 +40548,7 @@
         <v>12</v>
       </c>
       <c r="F471" t="n">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="G471" t="inlineStr"/>
       <c r="H471" t="n">
@@ -40632,7 +40632,7 @@
         <v>8</v>
       </c>
       <c r="F472" t="n">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="G472" t="inlineStr">
         <is>
@@ -40720,7 +40720,7 @@
         <v>6</v>
       </c>
       <c r="F473" t="n">
-        <v>1.6</v>
+        <v>2.6</v>
       </c>
       <c r="G473" t="inlineStr"/>
       <c r="H473" t="n">
@@ -40804,7 +40804,7 @@
         <v>1</v>
       </c>
       <c r="F474" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G474" t="inlineStr"/>
       <c r="H474" t="n">
@@ -40888,7 +40888,7 @@
         <v>23</v>
       </c>
       <c r="F475" t="n">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="G475" t="inlineStr">
         <is>
@@ -40976,7 +40976,7 @@
         <v>19</v>
       </c>
       <c r="F476" t="n">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="G476" t="inlineStr">
         <is>
@@ -41064,7 +41064,7 @@
         <v>10</v>
       </c>
       <c r="F477" t="n">
-        <v>1.6</v>
+        <v>2.7</v>
       </c>
       <c r="G477" t="inlineStr"/>
       <c r="H477" t="n">
@@ -41148,7 +41148,7 @@
         <v>8</v>
       </c>
       <c r="F478" t="n">
-        <v>2</v>
+        <v>2.934373349702772</v>
       </c>
       <c r="G478" t="inlineStr"/>
       <c r="H478" t="n">
@@ -41232,7 +41232,7 @@
         <v>3</v>
       </c>
       <c r="F479" t="n">
-        <v>1</v>
+        <v>2.897354275234529</v>
       </c>
       <c r="G479" t="inlineStr"/>
       <c r="H479" t="n">
@@ -41316,7 +41316,7 @@
         <v>9</v>
       </c>
       <c r="F480" t="n">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
       <c r="G480" t="inlineStr"/>
       <c r="H480" t="n">
@@ -41400,7 +41400,7 @@
         <v>1</v>
       </c>
       <c r="F481" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G481" t="inlineStr"/>
       <c r="H481" t="n">
@@ -41484,7 +41484,7 @@
         <v>1</v>
       </c>
       <c r="F482" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G482" t="inlineStr"/>
       <c r="H482" t="n">
@@ -41568,7 +41568,7 @@
         <v>9</v>
       </c>
       <c r="F483" t="n">
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="G483" t="inlineStr"/>
       <c r="H483" t="n">
@@ -41652,7 +41652,7 @@
         <v>9</v>
       </c>
       <c r="F484" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="G484" t="inlineStr"/>
       <c r="H484" t="n">
@@ -41736,7 +41736,7 @@
         <v>7</v>
       </c>
       <c r="F485" t="n">
-        <v>2</v>
+        <v>3.109789330019855</v>
       </c>
       <c r="G485" t="inlineStr">
         <is>
@@ -41824,7 +41824,7 @@
         <v>6</v>
       </c>
       <c r="F486" t="n">
-        <v>2</v>
+        <v>2.99622205531022</v>
       </c>
       <c r="G486" t="inlineStr">
         <is>
@@ -41912,7 +41912,7 @@
         <v>5</v>
       </c>
       <c r="F487" t="n">
-        <v>2</v>
+        <v>2.99622205531022</v>
       </c>
       <c r="G487" t="inlineStr">
         <is>
@@ -42000,7 +42000,7 @@
         <v>5</v>
       </c>
       <c r="F488" t="n">
-        <v>1</v>
+        <v>2.957872047908649</v>
       </c>
       <c r="G488" t="inlineStr">
         <is>
@@ -42088,7 +42088,7 @@
         <v>5</v>
       </c>
       <c r="F489" t="n">
-        <v>1</v>
+        <v>2.91913645020728</v>
       </c>
       <c r="G489" t="inlineStr">
         <is>
@@ -42176,7 +42176,7 @@
         <v>4</v>
       </c>
       <c r="F490" t="n">
-        <v>1.6</v>
+        <v>2.9</v>
       </c>
       <c r="G490" t="inlineStr"/>
       <c r="H490" t="n">
@@ -42260,7 +42260,7 @@
         <v>2</v>
       </c>
       <c r="F491" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G491" t="inlineStr"/>
       <c r="H491" t="n">
@@ -42344,7 +42344,7 @@
         <v>2</v>
       </c>
       <c r="F492" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G492" t="inlineStr">
         <is>
@@ -42432,7 +42432,7 @@
         <v>2</v>
       </c>
       <c r="F493" t="n">
-        <v>1</v>
+        <v>2.840120762128931</v>
       </c>
       <c r="G493" t="inlineStr"/>
       <c r="H493" t="n">
@@ -42516,7 +42516,7 @@
         <v>1</v>
       </c>
       <c r="F494" t="n">
-        <v>1</v>
+        <v>2.758316429348377</v>
       </c>
       <c r="G494" t="inlineStr"/>
       <c r="H494" t="n">
@@ -42600,7 +42600,7 @@
         <v>17</v>
       </c>
       <c r="F495" t="n">
-        <v>4</v>
+        <v>3.7</v>
       </c>
       <c r="G495" t="inlineStr"/>
       <c r="H495" t="n">
@@ -42684,7 +42684,7 @@
         <v>15</v>
       </c>
       <c r="F496" t="n">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="G496" t="inlineStr"/>
       <c r="H496" t="n">
@@ -42768,7 +42768,7 @@
         <v>6</v>
       </c>
       <c r="F497" t="n">
-        <v>1.3</v>
+        <v>2.6</v>
       </c>
       <c r="G497" t="inlineStr"/>
       <c r="H497" t="n">
@@ -42852,7 +42852,7 @@
         <v>5</v>
       </c>
       <c r="F498" t="n">
-        <v>2</v>
+        <v>2.951982378418139</v>
       </c>
       <c r="G498" t="inlineStr"/>
       <c r="H498" t="n">
@@ -42936,7 +42936,7 @@
         <v>3</v>
       </c>
       <c r="F499" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G499" t="inlineStr"/>
       <c r="H499" t="n">
@@ -43020,7 +43020,7 @@
         <v>2</v>
       </c>
       <c r="F500" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G500" t="inlineStr"/>
       <c r="H500" t="n">
@@ -43104,7 +43104,7 @@
         <v>2</v>
       </c>
       <c r="F501" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G501" t="inlineStr"/>
       <c r="H501" t="n">
@@ -43188,7 +43188,7 @@
         <v>1</v>
       </c>
       <c r="F502" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G502" t="inlineStr"/>
       <c r="H502" t="n">
@@ -43272,7 +43272,7 @@
         <v>13</v>
       </c>
       <c r="F503" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="G503" t="inlineStr">
         <is>
@@ -43360,7 +43360,7 @@
         <v>11</v>
       </c>
       <c r="F504" t="n">
-        <v>2</v>
+        <v>2.966802695515658</v>
       </c>
       <c r="G504" t="inlineStr">
         <is>
@@ -43448,7 +43448,7 @@
         <v>10</v>
       </c>
       <c r="F505" t="n">
-        <v>2</v>
+        <v>3.010990014781875</v>
       </c>
       <c r="G505" t="inlineStr">
         <is>
@@ -43536,7 +43536,7 @@
         <v>10</v>
       </c>
       <c r="F506" t="n">
-        <v>2</v>
+        <v>2.94511315530039</v>
       </c>
       <c r="G506" t="inlineStr"/>
       <c r="H506" t="n">
@@ -43620,7 +43620,7 @@
         <v>7</v>
       </c>
       <c r="F507" t="n">
-        <v>1.9</v>
+        <v>2.7</v>
       </c>
       <c r="G507" t="inlineStr"/>
       <c r="H507" t="n">
@@ -43704,7 +43704,7 @@
         <v>7</v>
       </c>
       <c r="F508" t="n">
-        <v>2</v>
+        <v>2.988764646508958</v>
       </c>
       <c r="G508" t="inlineStr">
         <is>
@@ -43792,7 +43792,7 @@
         <v>1</v>
       </c>
       <c r="F509" t="n">
-        <v>1</v>
+        <v>2.892140121749447</v>
       </c>
       <c r="G509" t="inlineStr"/>
       <c r="H509" t="n">
@@ -43876,7 +43876,7 @@
         <v>1</v>
       </c>
       <c r="F510" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G510" t="inlineStr"/>
       <c r="H510" t="n">
@@ -43960,7 +43960,7 @@
         <v>8</v>
       </c>
       <c r="F511" t="n">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="G511" t="inlineStr"/>
       <c r="H511" t="n">
@@ -44044,7 +44044,7 @@
         <v>1</v>
       </c>
       <c r="F512" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G512" t="inlineStr"/>
       <c r="H512" t="n">
@@ -44128,7 +44128,7 @@
         <v>1</v>
       </c>
       <c r="F513" t="n">
-        <v>1</v>
+        <v>2.923815989940977</v>
       </c>
       <c r="G513" t="inlineStr"/>
       <c r="H513" t="n">
@@ -44212,7 +44212,7 @@
         <v>11</v>
       </c>
       <c r="F514" t="n">
-        <v>4.3</v>
+        <v>3.8</v>
       </c>
       <c r="G514" t="inlineStr"/>
       <c r="H514" t="n">
@@ -44296,7 +44296,7 @@
         <v>9</v>
       </c>
       <c r="F515" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="G515" t="inlineStr"/>
       <c r="H515" t="n">
@@ -44380,7 +44380,7 @@
         <v>7</v>
       </c>
       <c r="F516" t="n">
-        <v>1.7</v>
+        <v>3</v>
       </c>
       <c r="G516" t="inlineStr"/>
       <c r="H516" t="n">
@@ -44464,7 +44464,7 @@
         <v>5</v>
       </c>
       <c r="F517" t="n">
-        <v>1.1</v>
+        <v>2.7</v>
       </c>
       <c r="G517" t="inlineStr"/>
       <c r="H517" t="n">
@@ -44548,7 +44548,7 @@
         <v>4</v>
       </c>
       <c r="F518" t="n">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="G518" t="inlineStr"/>
       <c r="H518" t="n">
@@ -44632,7 +44632,7 @@
         <v>3</v>
       </c>
       <c r="F519" t="n">
-        <v>1.1</v>
+        <v>2.7</v>
       </c>
       <c r="G519" t="inlineStr"/>
       <c r="H519" t="n">
@@ -44716,7 +44716,7 @@
         <v>3</v>
       </c>
       <c r="F520" t="n">
-        <v>1.3</v>
+        <v>2.6</v>
       </c>
       <c r="G520" t="inlineStr"/>
       <c r="H520" t="n">
@@ -44800,7 +44800,7 @@
         <v>2</v>
       </c>
       <c r="F521" t="n">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="G521" t="inlineStr"/>
       <c r="H521" t="n">
@@ -44884,7 +44884,7 @@
         <v>2</v>
       </c>
       <c r="F522" t="n">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="G522" t="inlineStr"/>
       <c r="H522" t="n">
@@ -44968,7 +44968,7 @@
         <v>2</v>
       </c>
       <c r="F523" t="n">
-        <v>1</v>
+        <v>2.879920376637045</v>
       </c>
       <c r="G523" t="inlineStr"/>
       <c r="H523" t="n">
@@ -45052,7 +45052,7 @@
         <v>14</v>
       </c>
       <c r="F524" t="n">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="G524" t="inlineStr">
         <is>
@@ -45140,7 +45140,7 @@
         <v>10</v>
       </c>
       <c r="F525" t="n">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="G525" t="inlineStr">
         <is>
@@ -45228,7 +45228,7 @@
         <v>9</v>
       </c>
       <c r="F526" t="n">
-        <v>2</v>
+        <v>3.038286869158483</v>
       </c>
       <c r="G526" t="inlineStr"/>
       <c r="H526" t="n">
@@ -45312,7 +45312,7 @@
         <v>8</v>
       </c>
       <c r="F527" t="n">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="G527" t="inlineStr"/>
       <c r="H527" t="n">
@@ -45396,7 +45396,7 @@
         <v>5</v>
       </c>
       <c r="F528" t="n">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="G528" t="inlineStr"/>
       <c r="H528" t="n">
@@ -45480,7 +45480,7 @@
         <v>5</v>
       </c>
       <c r="F529" t="n">
-        <v>1</v>
+        <v>2.929966981198159</v>
       </c>
       <c r="G529" t="inlineStr"/>
       <c r="H529" t="n">
@@ -45564,7 +45564,7 @@
         <v>4</v>
       </c>
       <c r="F530" t="n">
-        <v>1</v>
+        <v>2.885263000089072</v>
       </c>
       <c r="G530" t="inlineStr"/>
       <c r="H530" t="n">
@@ -45648,7 +45648,7 @@
         <v>3</v>
       </c>
       <c r="F531" t="n">
-        <v>2</v>
+        <v>3.038286869158483</v>
       </c>
       <c r="G531" t="inlineStr">
         <is>
@@ -45736,7 +45736,7 @@
         <v>3</v>
       </c>
       <c r="F532" t="n">
-        <v>1</v>
+        <v>2.885263000089072</v>
       </c>
       <c r="G532" t="inlineStr"/>
       <c r="H532" t="n">
@@ -45820,7 +45820,7 @@
         <v>2</v>
       </c>
       <c r="F533" t="n">
-        <v>1</v>
+        <v>2.862528910124882</v>
       </c>
       <c r="G533" t="inlineStr"/>
       <c r="H533" t="n">
@@ -45904,7 +45904,7 @@
         <v>1</v>
       </c>
       <c r="F534" t="n">
-        <v>1</v>
+        <v>2.79250473622765</v>
       </c>
       <c r="G534" t="inlineStr"/>
       <c r="H534" t="n">
@@ -45988,7 +45988,7 @@
         <v>14</v>
       </c>
       <c r="F535" t="n">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="G535" t="inlineStr"/>
       <c r="H535" t="n">
@@ -46072,7 +46072,7 @@
         <v>11</v>
       </c>
       <c r="F536" t="n">
-        <v>1.9</v>
+        <v>2.6</v>
       </c>
       <c r="G536" t="inlineStr"/>
       <c r="H536" t="n">
@@ -46156,7 +46156,7 @@
         <v>10</v>
       </c>
       <c r="F537" t="n">
-        <v>1.8</v>
+        <v>2.6</v>
       </c>
       <c r="G537" t="inlineStr">
         <is>
@@ -46244,7 +46244,7 @@
         <v>8</v>
       </c>
       <c r="F538" t="n">
-        <v>2.3</v>
+        <v>2.8</v>
       </c>
       <c r="G538" t="inlineStr">
         <is>
@@ -46332,7 +46332,7 @@
         <v>1</v>
       </c>
       <c r="F539" t="n">
-        <v>1</v>
+        <v>2.88694496126577</v>
       </c>
       <c r="G539" t="inlineStr"/>
       <c r="H539" t="n">
@@ -46416,7 +46416,7 @@
         <v>1</v>
       </c>
       <c r="F540" t="n">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="G540" t="inlineStr"/>
       <c r="H540" t="n">

</xml_diff>